<commit_message>
Presentando la clase final
</commit_message>
<xml_diff>
--- a/Semana 5/Tarea Opcional/Ejercicios Tarea Opcional-Finanzas Gerenciales.xlsx
+++ b/Semana 5/Tarea Opcional/Ejercicios Tarea Opcional-Finanzas Gerenciales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megam\Unitec\Master en Finanzas\Finanzas Gerenciales\Semana 10\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\megam\Unitec\Master en Finanzas\masterFinanzasFinanzasGerenciales\Semana 5\Tarea Opcional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF47A55D-6704-4A02-B69F-B5517D338C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37207A9A-DF67-420F-9BDA-98D32775B18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{15CD9A03-4508-4B95-8727-2AC2B5A225F6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" xr2:uid="{15CD9A03-4508-4B95-8727-2AC2B5A225F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Valor Presente de Flujos de Efe" sheetId="1" r:id="rId1"/>
@@ -235,15 +235,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>335280</xdr:colOff>
+      <xdr:colOff>36830</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>68580</xdr:rowOff>
+      <xdr:rowOff>125730</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>387350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>2540</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -258,8 +258,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="335280" y="68580"/>
-          <a:ext cx="4617720" cy="975360"/>
+          <a:off x="36830" y="125730"/>
+          <a:ext cx="6751320" cy="981710"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -465,16 +465,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>15240</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>589281</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>154940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>433137</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>93292</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>368301</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>53987</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -496,8 +496,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6850380" y="2026920"/>
-          <a:ext cx="5165157" cy="443812"/>
+          <a:off x="589281" y="1628140"/>
+          <a:ext cx="3093720" cy="267347"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -814,28 +814,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42F67D5E-D9DC-4F68-B46D-CAD11C02E2B4}">
-  <dimension ref="B8:R22"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B8:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H1" sqref="A1:H43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.453125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>0</v>
       </c>
@@ -843,7 +846,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <v>1</v>
       </c>
@@ -851,7 +854,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>2</v>
       </c>
@@ -859,7 +862,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <v>3</v>
       </c>
@@ -867,7 +870,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" s="2">
         <v>4</v>
       </c>
@@ -875,18 +878,12 @@
         <v>1075</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N15" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" s="10" t="s">
         <v>0</v>
       </c>
@@ -902,38 +899,8 @@
       <c r="F17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H17" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="L17" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="N17" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="O17" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="P17" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q17" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="R17" s="10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" s="2">
         <v>1</v>
       </c>
@@ -951,42 +918,8 @@
         <f>E18*C18</f>
         <v>863.63636363636363</v>
       </c>
-      <c r="H18" s="2">
-        <v>1</v>
-      </c>
-      <c r="I18" s="3">
-        <v>950</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="8">
-        <f>1/(1+0.18)^H18</f>
-        <v>0.84745762711864414</v>
-      </c>
-      <c r="L18" s="6">
-        <f>K18*I18</f>
-        <v>805.08474576271192</v>
-      </c>
-      <c r="N18" s="2">
-        <v>1</v>
-      </c>
-      <c r="O18" s="3">
-        <v>950</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="Q18" s="8">
-        <f>1/(1+0.24)^N18</f>
-        <v>0.80645161290322587</v>
-      </c>
-      <c r="R18" s="6">
-        <f>Q18*O18</f>
-        <v>766.12903225806463</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>2</v>
       </c>
@@ -1004,42 +937,8 @@
         <f t="shared" ref="F19:F21" si="1">E19*C19</f>
         <v>859.50413223140481</v>
       </c>
-      <c r="H19" s="2">
-        <v>2</v>
-      </c>
-      <c r="I19" s="3">
-        <v>1040</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K19" s="8">
-        <f t="shared" ref="K19:K21" si="2">1/(1+0.18)^H19</f>
-        <v>0.71818442976156283</v>
-      </c>
-      <c r="L19" s="6">
-        <f t="shared" ref="L19:L21" si="3">K19*I19</f>
-        <v>746.91180695202536</v>
-      </c>
-      <c r="N19" s="2">
-        <v>2</v>
-      </c>
-      <c r="O19" s="3">
-        <v>1040</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q19" s="8">
-        <f t="shared" ref="Q19:Q21" si="4">1/(1+0.24)^N19</f>
-        <v>0.65036420395421435</v>
-      </c>
-      <c r="R19" s="6">
-        <f t="shared" ref="R19:R21" si="5">Q19*O19</f>
-        <v>676.37877211238288</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>3</v>
       </c>
@@ -1057,42 +956,8 @@
         <f t="shared" si="1"/>
         <v>848.98572501878266</v>
       </c>
-      <c r="H20" s="2">
-        <v>3</v>
-      </c>
-      <c r="I20" s="3">
-        <v>1130</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K20" s="8">
-        <f t="shared" si="2"/>
-        <v>0.6086308726792905</v>
-      </c>
-      <c r="L20" s="6">
-        <f t="shared" si="3"/>
-        <v>687.75288612759823</v>
-      </c>
-      <c r="N20" s="2">
-        <v>3</v>
-      </c>
-      <c r="O20" s="3">
-        <v>1130</v>
-      </c>
-      <c r="P20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q20" s="8">
-        <f t="shared" si="4"/>
-        <v>0.52448726125339862</v>
-      </c>
-      <c r="R20" s="6">
-        <f t="shared" si="5"/>
-        <v>592.67060521634039</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B21" s="2">
         <v>4</v>
       </c>
@@ -1110,42 +975,8 @@
         <f t="shared" si="1"/>
         <v>734.23946451745076</v>
       </c>
-      <c r="H21" s="2">
-        <v>4</v>
-      </c>
-      <c r="I21" s="3">
-        <v>1075</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K21" s="8">
-        <f t="shared" si="2"/>
-        <v>0.51578887515194116</v>
-      </c>
-      <c r="L21" s="6">
-        <f t="shared" si="3"/>
-        <v>554.47304078833679</v>
-      </c>
-      <c r="N21" s="2">
-        <v>4</v>
-      </c>
-      <c r="O21" s="3">
-        <v>1075</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q21" s="8">
-        <f t="shared" si="4"/>
-        <v>0.42297359778499888</v>
-      </c>
-      <c r="R21" s="6">
-        <f t="shared" si="5"/>
-        <v>454.6966176188738</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
@@ -1153,42 +984,245 @@
         <f>SUM(F18:F21)</f>
         <v>3306.3656854040019</v>
       </c>
-      <c r="H22" s="4" t="s">
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="3">
+        <v>950</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="8">
+        <f>1/(1+0.18)^B28</f>
+        <v>0.84745762711864414</v>
+      </c>
+      <c r="F28" s="6">
+        <f>E28*C28</f>
+        <v>805.08474576271192</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1040</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="8">
+        <f t="shared" ref="E29:E31" si="2">1/(1+0.18)^B29</f>
+        <v>0.71818442976156283</v>
+      </c>
+      <c r="F29" s="6">
+        <f t="shared" ref="F29:F31" si="3">E29*C29</f>
+        <v>746.91180695202536</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="2">
+        <v>3</v>
+      </c>
+      <c r="C30" s="3">
+        <v>1130</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="8">
+        <f t="shared" si="2"/>
+        <v>0.6086308726792905</v>
+      </c>
+      <c r="F30" s="6">
+        <f t="shared" si="3"/>
+        <v>687.75288612759823</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="2">
+        <v>4</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1075</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="8">
+        <f t="shared" si="2"/>
+        <v>0.51578887515194116</v>
+      </c>
+      <c r="F31" s="6">
+        <f t="shared" si="3"/>
+        <v>554.47304078833679</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L22" s="7">
-        <f>SUM(L18:L21)</f>
+      <c r="F32" s="7">
+        <f>SUM(F28:F31)</f>
         <v>2794.2224796306723</v>
       </c>
-      <c r="N22" s="4" t="s">
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B35" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="3">
+        <v>950</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="8">
+        <f>1/(1+0.24)^B38</f>
+        <v>0.80645161290322587</v>
+      </c>
+      <c r="F38" s="6">
+        <f>E38*C38</f>
+        <v>766.12903225806463</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B39" s="2">
+        <v>2</v>
+      </c>
+      <c r="C39" s="3">
+        <v>1040</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="8">
+        <f t="shared" ref="E39:E41" si="4">1/(1+0.24)^B39</f>
+        <v>0.65036420395421435</v>
+      </c>
+      <c r="F39" s="6">
+        <f t="shared" ref="F39:F41" si="5">E39*C39</f>
+        <v>676.37877211238288</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B40" s="2">
+        <v>3</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1130</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E40" s="8">
+        <f t="shared" si="4"/>
+        <v>0.52448726125339862</v>
+      </c>
+      <c r="F40" s="6">
+        <f t="shared" si="5"/>
+        <v>592.67060521634039</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B41" s="2">
+        <v>4</v>
+      </c>
+      <c r="C41" s="3">
+        <v>1075</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="8">
+        <f t="shared" si="4"/>
+        <v>0.42297359778499888</v>
+      </c>
+      <c r="F41" s="6">
+        <f t="shared" si="5"/>
+        <v>454.6966176188738</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="R22" s="7">
-        <f>SUM(R18:R21)</f>
+      <c r="F42" s="7">
+        <f>SUM(F38:F41)</f>
         <v>2489.8750272056618</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD30DBC7-F9D4-449A-9D8A-62826578129B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="B12:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="K17" sqref="A1:K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>22</v>
       </c>
@@ -1196,7 +1230,7 @@
         <v>68500</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>23</v>
       </c>
@@ -1204,7 +1238,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
     </row>
-    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>24</v>
       </c>
@@ -1212,7 +1246,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>21</v>
       </c>
@@ -1220,20 +1254,21 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="4">
         <f>68500/((1-(1/(1+(0.069/12))^60))/(0.069/12))</f>
         <v>1353.1525873258461</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
       <c r="C19" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup scale="90" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>